<commit_message>
feat: add search in browser
</commit_message>
<xml_diff>
--- a/tests/result.xlsx
+++ b/tests/result.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,40 +460,45 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>Nome do anunciante</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>Preço</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Endereço</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Área</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Quartos</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Banheiros</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Vagas</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Data da publicação</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Link</t>
         </is>
@@ -518,30 +523,35 @@
       <c r="D2" t="n">
         <v>11998835264</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Richard</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
         <v>500000</v>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>Estrada Municipal Waldomiro Fregnhami 551, Nova Monte Serrat</t>
         </is>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>50</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>2</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>1</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>0</v>
       </c>
-      <c r="K2" s="2" t="n">
+      <c r="L2" s="2" t="n">
         <v>44990</v>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>https://www.zapimoveis.com.br/imovel/venda-apartamento-2-quartos-mobiliado-pacaembu-itupeva-sp-51m2-id-2621400516/</t>
         </is>

</xml_diff>